<commit_message>
new commit for xslt report,log4j etc
</commit_message>
<xml_diff>
--- a/tc.xlsx
+++ b/tc.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>TC ID</t>
   </si>
@@ -76,7 +76,7 @@
     <t>Afrin@1996</t>
   </si>
   <si>
-    <t>abc@gmail.com</t>
+    <t>acd@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -506,6 +506,9 @@
       <c r="B5" t="s">
         <v>11</v>
       </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
       <c r="D5" t="s">
         <v>6</v>
       </c>

</xml_diff>